<commit_message>
Updated control signals in excel file
</commit_message>
<xml_diff>
--- a/docs/Instructions_details.xlsx
+++ b/docs/Instructions_details.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NADA\Desktop\CCE sem 4\comp Architecture\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Muhab\OneDrive\Documents\GitHub\Pipelined-Von-Neumann-Processor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B04D4F-CCC3-41B7-85E8-2EF8024E12E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="1"/>
+    <workbookView xWindow="7200" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpCode" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="100">
   <si>
     <t>Instruction</t>
   </si>
@@ -276,52 +277,61 @@
     <t>11</t>
   </si>
   <si>
+    <t>ccr_wr_en</t>
+  </si>
+  <si>
+    <t>reg_write</t>
+  </si>
+  <si>
+    <t>alu_src</t>
+  </si>
+  <si>
+    <t>pc_src</t>
+  </si>
+  <si>
+    <t>int_en</t>
+  </si>
+  <si>
+    <t>return_en</t>
+  </si>
+  <si>
+    <t>Opcode</t>
+  </si>
+  <si>
+    <t>1/0</t>
+  </si>
+  <si>
+    <t>1 bit for the index</t>
+  </si>
+  <si>
+    <t>16 bits</t>
+  </si>
+  <si>
+    <t>5 bits</t>
+  </si>
+  <si>
+    <t>30 bits</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>ccr_wr_en</t>
-  </si>
-  <si>
-    <t>reg_write</t>
-  </si>
-  <si>
-    <t>alu_src</t>
-  </si>
-  <si>
-    <t>pc_src</t>
-  </si>
-  <si>
-    <t>int_en</t>
-  </si>
-  <si>
-    <t>return_en</t>
-  </si>
-  <si>
-    <t>Opcode</t>
-  </si>
-  <si>
-    <t>1/0</t>
-  </si>
-  <si>
-    <t>1 bit for the index</t>
-  </si>
-  <si>
-    <t>16 bits</t>
-  </si>
-  <si>
-    <t>5 bits</t>
-  </si>
-  <si>
-    <t>30 bits</t>
+    <t>x/0</t>
+  </si>
+  <si>
+    <t>x/00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -470,9 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -485,6 +492,12 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,29 +816,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="59" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="6" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
     <col min="17" max="17" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -833,13 +847,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>74</v>
@@ -863,7 +877,7 @@
         <v>77</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>6</v>
@@ -875,13 +889,13 @@
         <v>73</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -895,7 +909,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -908,14 +922,14 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>65</v>
+      <c r="E3" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="16" t="s">
-        <v>65</v>
+      <c r="G3" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>65</v>
@@ -930,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -939,10 +953,10 @@
         <v>0</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -951,7 +965,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -964,14 +978,14 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>65</v>
+      <c r="E4" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>65</v>
+      <c r="G4" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>65</v>
@@ -986,19 +1000,19 @@
         <v>0</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P4" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -1007,7 +1021,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1020,14 +1034,14 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>65</v>
+      <c r="E5" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>65</v>
+      <c r="G5" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>65</v>
@@ -1042,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -1051,10 +1065,10 @@
         <v>0</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1063,7 +1077,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1076,14 +1090,14 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>65</v>
+      <c r="E6" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>65</v>
+      <c r="G6" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>65</v>
@@ -1098,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -1107,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P6" s="16">
         <v>0</v>
@@ -1119,7 +1133,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1132,14 +1146,14 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>65</v>
+      <c r="E7" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>65</v>
+      <c r="G7" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>65</v>
@@ -1154,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -1163,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P7" s="16">
         <v>1</v>
@@ -1175,7 +1189,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
@@ -1185,7 +1199,7 @@
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1204,8 +1218,8 @@
       <c r="F9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>65</v>
+      <c r="G9" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>65</v>
@@ -1229,10 +1243,10 @@
         <v>0</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P9" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1241,7 +1255,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1260,8 +1274,8 @@
       <c r="F10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>65</v>
+      <c r="G10" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>64</v>
@@ -1285,10 +1299,10 @@
         <v>0</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P10" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1297,7 +1311,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1316,8 +1330,8 @@
       <c r="F11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>65</v>
+      <c r="G11" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H11" s="16" t="s">
         <v>65</v>
@@ -1332,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1341,10 +1355,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1353,7 +1367,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1373,7 +1387,7 @@
         <v>47</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>64</v>
@@ -1388,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1397,10 +1411,10 @@
         <v>0</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1409,7 +1423,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1429,7 +1443,7 @@
         <v>48</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>65</v>
@@ -1444,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1453,10 +1467,10 @@
         <v>0</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P13" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1465,7 +1479,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1484,8 +1498,8 @@
       <c r="F14" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="16" t="s">
-        <v>65</v>
+      <c r="G14" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>65</v>
@@ -1500,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1509,10 +1523,10 @@
         <v>0</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q14">
         <v>1</v>
@@ -1521,14 +1535,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>80</v>
       </c>
       <c r="D15">
@@ -1540,8 +1554,8 @@
       <c r="F15" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>65</v>
+      <c r="G15" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>64</v>
@@ -1564,11 +1578,11 @@
       <c r="N15" s="12">
         <v>0</v>
       </c>
-      <c r="O15" s="17" t="s">
-        <v>65</v>
+      <c r="O15" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -1577,7 +1591,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1585,7 +1599,7 @@
         <v>70</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1596,8 +1610,8 @@
       <c r="F16" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="16" t="s">
-        <v>65</v>
+      <c r="G16" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H16" s="16" t="s">
         <v>64</v>
@@ -1621,10 +1635,10 @@
         <v>0</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P16" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1633,18 +1647,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="7" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" s="7" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="F17" s="14"/>
-      <c r="H17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1663,8 +1677,8 @@
       <c r="F18" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>65</v>
+      <c r="G18" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H18" s="16" t="s">
         <v>64</v>
@@ -1688,10 +1702,10 @@
         <v>0</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P18" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -1700,7 +1714,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1719,8 +1733,8 @@
       <c r="F19" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>65</v>
+      <c r="G19" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="H19" s="16" t="s">
         <v>64</v>
@@ -1744,10 +1758,10 @@
         <v>0</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P19" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -1756,7 +1770,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1775,8 +1789,8 @@
       <c r="F20" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>65</v>
+      <c r="G20" s="16">
+        <v>0</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>64</v>
@@ -1800,10 +1814,10 @@
         <v>0</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P20" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -1812,7 +1826,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1831,8 +1845,8 @@
       <c r="F21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>65</v>
+      <c r="G21" s="16">
+        <v>0</v>
       </c>
       <c r="H21" s="16" t="s">
         <v>64</v>
@@ -1856,10 +1870,10 @@
         <v>0</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P21" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -1868,7 +1882,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1887,8 +1901,8 @@
       <c r="F22" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="16" t="s">
-        <v>65</v>
+      <c r="G22" s="16">
+        <v>0</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>64</v>
@@ -1912,10 +1926,10 @@
         <v>0</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P22" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -1924,18 +1938,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="7" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" s="7" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="F23" s="14"/>
-      <c r="H23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-    </row>
-    <row r="24" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+    </row>
+    <row r="24" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>14</v>
       </c>
@@ -1948,8 +1962,8 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>65</v>
+      <c r="E24" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>50</v>
@@ -1970,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M24" s="12">
         <v>0</v>
@@ -1982,7 +1996,7 @@
         <v>76</v>
       </c>
       <c r="P24" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -1991,7 +2005,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -2004,8 +2018,8 @@
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25" s="16" t="s">
-        <v>65</v>
+      <c r="E25" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>51</v>
@@ -2026,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -2038,7 +2052,7 @@
         <v>75</v>
       </c>
       <c r="P25" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -2047,7 +2061,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -2060,8 +2074,8 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>65</v>
+      <c r="E26" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>52</v>
@@ -2082,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -2094,7 +2108,7 @@
         <v>10</v>
       </c>
       <c r="P26" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -2103,7 +2117,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -2116,8 +2130,8 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>65</v>
+      <c r="E27" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>53</v>
@@ -2138,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -2150,7 +2164,7 @@
         <v>11</v>
       </c>
       <c r="P27" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -2159,25 +2173,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="7" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" s="7" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
       <c r="F28" s="14"/>
-      <c r="H28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-    </row>
-    <row r="29" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+    </row>
+    <row r="29" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="19" t="s">
         <v>80</v>
       </c>
       <c r="D29">
@@ -2192,7 +2206,7 @@
       <c r="G29">
         <v>1</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="18" t="s">
         <v>64</v>
       </c>
       <c r="I29">
@@ -2214,10 +2228,10 @@
         <v>0</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P29" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -2226,7 +2240,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2248,7 +2262,7 @@
       <c r="G30">
         <v>1</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="18" t="s">
         <v>64</v>
       </c>
       <c r="I30">
@@ -2270,10 +2284,10 @@
         <v>0</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P30" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -2282,7 +2296,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2304,7 +2318,7 @@
       <c r="G31">
         <v>1</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="18" t="s">
         <v>64</v>
       </c>
       <c r="I31">
@@ -2326,10 +2340,10 @@
         <v>0</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P31" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -2338,7 +2352,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -2360,7 +2374,7 @@
       <c r="G32">
         <v>1</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="18" t="s">
         <v>64</v>
       </c>
       <c r="I32">
@@ -2382,10 +2396,10 @@
         <v>0</v>
       </c>
       <c r="O32" s="16" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="P32" s="16" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="Q32">
         <v>0</v>
@@ -2394,17 +2408,19 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="H33" s="11"/>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="23"/>
       <c r="O33" s="16"/>
     </row>
-    <row r="34" spans="8:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
       <c r="H34" s="11"/>
     </row>
-    <row r="35" spans="8:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="8:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
       <c r="H36" s="11"/>
     </row>
   </sheetData>
@@ -2415,56 +2431,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection sqref="A1:G33"/>
+    <sheetView zoomScale="76" workbookViewId="0">
+      <selection activeCell="E2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="23" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="23" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2484,7 +2500,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2504,7 +2520,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2524,7 +2540,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2545,7 +2561,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2566,26 +2582,26 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>94</v>
+      <c r="F9" s="22" t="s">
+        <v>92</v>
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2606,7 +2622,7 @@
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2627,7 +2643,7 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2648,7 +2664,7 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2669,7 +2685,7 @@
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2690,15 +2706,15 @@
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>92</v>
+      <c r="C15" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="D15" t="s">
         <v>65</v>
@@ -2706,11 +2722,11 @@
       <c r="E15" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2730,7 +2746,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2750,25 +2766,25 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -2788,7 +2804,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -2808,7 +2824,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2828,7 +2844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2848,7 +2864,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2868,25 +2884,25 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2906,7 +2922,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2926,7 +2942,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -2946,7 +2962,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -2966,25 +2982,25 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3004,7 +3020,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -3024,7 +3040,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -3044,7 +3060,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3071,6 +3087,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010098146755E301CC4CA0BF2C65E31301A5" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="52b6ddeebc1cb55ae93faaec169ffd15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e6e36e7f-f981-45b8-86e3-dec104a3a742" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="65e6098583fe78a92ca391fc534c320c" ns3:_="">
     <xsd:import namespace="e6e36e7f-f981-45b8-86e3-dec104a3a742"/>
@@ -3216,22 +3247,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04213643-6433-454F-89B7-5E82788C4828}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="e6e36e7f-f981-45b8-86e3-dec104a3a742"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47076F1B-9036-4235-8567-538FF8DCA084}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCB7562-BBB4-43A7-A298-3132544BFB4D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3247,28 +3287,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47076F1B-9036-4235-8567-538FF8DCA084}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04213643-6433-454F-89B7-5E82788C4828}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="e6e36e7f-f981-45b8-86e3-dec104a3a742"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>